<commit_message>
UP TO PROPERTY FILE
</commit_message>
<xml_diff>
--- a/api_handler_app/Habile_Investak_API_Dictionary.xlsx
+++ b/api_handler_app/Habile_Investak_API_Dictionary.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3721" uniqueCount="1352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3728" uniqueCount="1352">
   <si>
     <t>DESCRIPTION</t>
   </si>
@@ -4424,7 +4424,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -4619,6 +4619,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4626,498 +4629,6 @@
     <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
   <dxfs count="116">
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -6297,6 +5808,498 @@
         <name val="Segoe UI"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -7673,16 +7676,16 @@
   </sortState>
   <tableColumns count="11">
     <tableColumn id="1" name="#"/>
-    <tableColumn id="2" name="API NAME " dataDxfId="26"/>
-    <tableColumn id="3" name="DATE" dataDxfId="25"/>
-    <tableColumn id="4" name="VERSION #" dataDxfId="24"/>
-    <tableColumn id="5" name="API #" dataDxfId="23"/>
-    <tableColumn id="6" name="HANDLER DATE" dataDxfId="22"/>
-    <tableColumn id="7" name="LIST OF CHANGES" dataDxfId="21"/>
-    <tableColumn id="8" name="CHAPTER" dataDxfId="20"/>
-    <tableColumn id="11" name="API IMPACTED" dataDxfId="19"/>
-    <tableColumn id="9" name="IMPACT" dataDxfId="18"/>
-    <tableColumn id="10" name="SOLUTION" dataDxfId="17"/>
+    <tableColumn id="2" name="API NAME " dataDxfId="9"/>
+    <tableColumn id="3" name="DATE" dataDxfId="8"/>
+    <tableColumn id="4" name="VERSION #" dataDxfId="7"/>
+    <tableColumn id="5" name="API #" dataDxfId="6"/>
+    <tableColumn id="6" name="HANDLER DATE" dataDxfId="5"/>
+    <tableColumn id="7" name="LIST OF CHANGES" dataDxfId="4"/>
+    <tableColumn id="8" name="CHAPTER" dataDxfId="3"/>
+    <tableColumn id="11" name="API IMPACTED" dataDxfId="2"/>
+    <tableColumn id="9" name="IMPACT" dataDxfId="1"/>
+    <tableColumn id="10" name="SOLUTION" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7722,8 +7725,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:M30" totalsRowShown="0" headerRowDxfId="89" dataDxfId="88" tableBorderDxfId="87">
-  <autoFilter ref="A1:M30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:M31" totalsRowShown="0" headerRowDxfId="89" dataDxfId="88" tableBorderDxfId="87">
+  <autoFilter ref="A1:M31">
     <filterColumn colId="4"/>
     <filterColumn colId="6">
       <customFilters>
@@ -7770,35 +7773,31 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:L107" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3" headerRowBorderDxfId="1" tableBorderDxfId="2" totalsRowBorderDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:L107" totalsRowShown="0" headerRowDxfId="62" dataDxfId="60" headerRowBorderDxfId="61" tableBorderDxfId="59" totalsRowBorderDxfId="58">
   <autoFilter ref="A1:L107">
     <filterColumn colId="1"/>
-    <filterColumn colId="6">
-      <filters>
-        <filter val="DateTime"/>
-      </filters>
-    </filterColumn>
+    <filterColumn colId="6"/>
   </autoFilter>
   <tableColumns count="12">
-    <tableColumn id="1" name="#" dataDxfId="16"/>
-    <tableColumn id="2" name="API NAME" dataDxfId="15"/>
-    <tableColumn id="3" name="SNO" dataDxfId="14"/>
-    <tableColumn id="4" name="PARAMETER" dataDxfId="13"/>
-    <tableColumn id="5" name="DESCRIPTION" dataDxfId="12"/>
-    <tableColumn id="6" name="BUSINESS_TAG" dataDxfId="11"/>
-    <tableColumn id="7" name="Data Type " dataDxfId="10"/>
-    <tableColumn id="8" name="VALID VALUES" dataDxfId="9"/>
-    <tableColumn id="9" name="MANDATORY" dataDxfId="8"/>
-    <tableColumn id="10" name="DEFAULT" dataDxfId="7"/>
-    <tableColumn id="11" name="TRANSFORMATION" dataDxfId="6"/>
-    <tableColumn id="12" name="INVESTAK SCREEN  FIELD / SAMPLE" dataDxfId="5"/>
+    <tableColumn id="1" name="#" dataDxfId="57"/>
+    <tableColumn id="2" name="API NAME" dataDxfId="56"/>
+    <tableColumn id="3" name="SNO" dataDxfId="55"/>
+    <tableColumn id="4" name="PARAMETER" dataDxfId="54"/>
+    <tableColumn id="5" name="DESCRIPTION" dataDxfId="53"/>
+    <tableColumn id="6" name="BUSINESS_TAG" dataDxfId="52"/>
+    <tableColumn id="7" name="Data Type " dataDxfId="51"/>
+    <tableColumn id="8" name="VALID VALUES" dataDxfId="50"/>
+    <tableColumn id="9" name="MANDATORY" dataDxfId="49"/>
+    <tableColumn id="10" name="DEFAULT" dataDxfId="48"/>
+    <tableColumn id="11" name="TRANSFORMATION" dataDxfId="47"/>
+    <tableColumn id="12" name="INVESTAK SCREEN  FIELD / SAMPLE" dataDxfId="46"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:K273" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61" tableBorderDxfId="60">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:K273" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44" tableBorderDxfId="43">
   <autoFilter ref="A1:K273">
     <filterColumn colId="1"/>
     <filterColumn colId="6">
@@ -7809,42 +7808,42 @@
     <filterColumn colId="8"/>
   </autoFilter>
   <tableColumns count="11">
-    <tableColumn id="1" name="#" dataDxfId="59"/>
-    <tableColumn id="2" name="API NAME" dataDxfId="58"/>
-    <tableColumn id="3" name="SNO" dataDxfId="57"/>
-    <tableColumn id="4" name="PARAMETER" dataDxfId="56"/>
-    <tableColumn id="5" name="DESCRIPTION" dataDxfId="55"/>
-    <tableColumn id="6" name="BUSINESS_TAG" dataDxfId="54"/>
-    <tableColumn id="7" name="DATA _TYPE" dataDxfId="53"/>
-    <tableColumn id="8" name="VALID VALUES" dataDxfId="52"/>
-    <tableColumn id="11" name="OPTIONAL" dataDxfId="51"/>
-    <tableColumn id="10" name="TRANSFORMATION" dataDxfId="50"/>
-    <tableColumn id="9" name="SPECIAL PROCESS" dataDxfId="49"/>
+    <tableColumn id="1" name="#" dataDxfId="42"/>
+    <tableColumn id="2" name="API NAME" dataDxfId="41"/>
+    <tableColumn id="3" name="SNO" dataDxfId="40"/>
+    <tableColumn id="4" name="PARAMETER" dataDxfId="39"/>
+    <tableColumn id="5" name="DESCRIPTION" dataDxfId="38"/>
+    <tableColumn id="6" name="BUSINESS_TAG" dataDxfId="37"/>
+    <tableColumn id="7" name="DATA _TYPE" dataDxfId="36"/>
+    <tableColumn id="8" name="VALID VALUES" dataDxfId="35"/>
+    <tableColumn id="11" name="OPTIONAL" dataDxfId="34"/>
+    <tableColumn id="10" name="TRANSFORMATION" dataDxfId="33"/>
+    <tableColumn id="9" name="SPECIAL PROCESS" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:G119" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47" tableBorderDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:G119" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30" tableBorderDxfId="29">
   <autoFilter ref="A1:G119">
     <filterColumn colId="1"/>
   </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" name="#" dataDxfId="45"/>
-    <tableColumn id="2" name="API NAME" dataDxfId="44"/>
-    <tableColumn id="3" name="SNO" dataDxfId="43"/>
-    <tableColumn id="4" name="PARAMETER" dataDxfId="42"/>
-    <tableColumn id="5" name="DESCRIPTION" dataDxfId="41"/>
-    <tableColumn id="6" name="Data Type " dataDxfId="40"/>
-    <tableColumn id="7" name="VALID VALUES" dataDxfId="39"/>
+    <tableColumn id="1" name="#" dataDxfId="28"/>
+    <tableColumn id="2" name="API NAME" dataDxfId="27"/>
+    <tableColumn id="3" name="SNO" dataDxfId="26"/>
+    <tableColumn id="4" name="PARAMETER" dataDxfId="25"/>
+    <tableColumn id="5" name="DESCRIPTION" dataDxfId="24"/>
+    <tableColumn id="6" name="Data Type " dataDxfId="23"/>
+    <tableColumn id="7" name="VALID VALUES" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:G133" totalsRowShown="0" headerRowDxfId="38" dataDxfId="36" headerRowBorderDxfId="37" tableBorderDxfId="35" totalsRowBorderDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:G133" totalsRowShown="0" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18" totalsRowBorderDxfId="17">
   <autoFilter ref="A1:G133">
     <filterColumn colId="1">
       <filters>
@@ -7857,13 +7856,13 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" name="#" dataDxfId="33"/>
-    <tableColumn id="2" name="ARRAY NAME" dataDxfId="32"/>
-    <tableColumn id="3" name="SNO" dataDxfId="31"/>
-    <tableColumn id="4" name="PARAMETER" dataDxfId="30"/>
-    <tableColumn id="5" name="DESCRIPTION" dataDxfId="29"/>
-    <tableColumn id="6" name="Data Type " dataDxfId="28"/>
-    <tableColumn id="7" name="VALID VALUES" dataDxfId="27"/>
+    <tableColumn id="1" name="#" dataDxfId="16"/>
+    <tableColumn id="2" name="ARRAY NAME" dataDxfId="15"/>
+    <tableColumn id="3" name="SNO" dataDxfId="14"/>
+    <tableColumn id="4" name="PARAMETER" dataDxfId="13"/>
+    <tableColumn id="5" name="DESCRIPTION" dataDxfId="12"/>
+    <tableColumn id="6" name="Data Type " dataDxfId="11"/>
+    <tableColumn id="7" name="VALID VALUES" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8158,7 +8157,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -9600,13 +9599,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N30"/>
+  <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G32" sqref="G32"/>
+      <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9614,7 +9613,7 @@
     <col min="1" max="1" width="5.28515625" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" customWidth="1"/>
     <col min="4" max="4" width="6.5703125" customWidth="1"/>
-    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="5" max="5" width="21.28515625" customWidth="1"/>
     <col min="6" max="6" width="17.42578125" customWidth="1"/>
     <col min="7" max="7" width="41.42578125" customWidth="1"/>
     <col min="8" max="8" width="79.140625" customWidth="1"/>
@@ -9749,9 +9748,9 @@
         <v>180</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="24">
+    <row r="4" spans="1:14">
       <c r="A4" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>137</v>
@@ -9759,38 +9758,32 @@
       <c r="C4" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="D4" s="5">
-        <v>3.3</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="G4" s="56" t="s">
-        <v>1290</v>
-      </c>
-      <c r="H4" t="s">
-        <v>1259</v>
+      <c r="D4" s="68">
+        <v>3.2</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="F4" s="68"/>
+      <c r="G4" s="68"/>
+      <c r="H4" s="49" t="s">
+        <v>1258</v>
       </c>
       <c r="I4" s="6" t="s">
         <v>1231</v>
       </c>
-      <c r="J4" s="5" t="s">
-        <v>1232</v>
+      <c r="J4" s="6" t="s">
+        <v>1231</v>
       </c>
       <c r="K4" s="5" t="s">
         <v>1232</v>
       </c>
-      <c r="L4" s="6"/>
-      <c r="M4" s="15" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="36" hidden="1">
+      <c r="L4" s="68"/>
+      <c r="M4" s="53"/>
+    </row>
+    <row r="5" spans="1:14" ht="24">
       <c r="A5" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>137</v>
@@ -9799,72 +9792,72 @@
         <v>83</v>
       </c>
       <c r="D5" s="5">
-        <v>3.4</v>
+        <v>3.3</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>171</v>
+        <v>88</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="G5" s="6"/>
+        <v>89</v>
+      </c>
+      <c r="G5" s="56" t="s">
+        <v>1290</v>
+      </c>
       <c r="H5" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
       <c r="I5" s="6" t="s">
+        <v>1231</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>1232</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>1232</v>
+      </c>
+      <c r="L5" s="6"/>
+      <c r="M5" s="15" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="36" hidden="1">
+      <c r="A6" s="5">
         <v>4</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="L5" s="5"/>
-      <c r="M5" s="15"/>
-    </row>
-    <row r="6" spans="1:14" ht="48">
-      <c r="A6" s="5">
-        <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>137</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="D6" s="5">
-        <v>4.0999999999999996</v>
+        <v>3.4</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>91</v>
+        <v>171</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="G6" s="56" t="s">
-        <v>1291</v>
-      </c>
-      <c r="H6" s="50" t="s">
-        <v>1261</v>
+        <v>172</v>
+      </c>
+      <c r="G6" s="6"/>
+      <c r="H6" t="s">
+        <v>1260</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>1231</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>1231</v>
-      </c>
-      <c r="K6" s="6" t="s">
-        <v>177</v>
+        <v>4</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>148</v>
       </c>
       <c r="L6" s="5"/>
-      <c r="M6" s="16" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="36">
+      <c r="M6" s="15"/>
+    </row>
+    <row r="7" spans="1:14" ht="48">
       <c r="A7" s="5">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>137</v>
@@ -9873,19 +9866,19 @@
         <v>90</v>
       </c>
       <c r="D7" s="5">
-        <v>4.2</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>1292</v>
-      </c>
-      <c r="H7" t="s">
-        <v>1262</v>
+        <v>92</v>
+      </c>
+      <c r="G7" s="56" t="s">
+        <v>1291</v>
+      </c>
+      <c r="H7" s="50" t="s">
+        <v>1261</v>
       </c>
       <c r="I7" s="6" t="s">
         <v>1231</v>
@@ -9897,13 +9890,13 @@
         <v>177</v>
       </c>
       <c r="L7" s="5"/>
-      <c r="M7" s="15" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="108">
+      <c r="M7" s="16" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="36">
       <c r="A8" s="5">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>137</v>
@@ -9912,19 +9905,19 @@
         <v>90</v>
       </c>
       <c r="D8" s="5">
-        <v>4.3</v>
+        <v>4.2</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="H8" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="I8" s="6" t="s">
         <v>1231</v>
@@ -9932,17 +9925,17 @@
       <c r="J8" s="6" t="s">
         <v>1231</v>
       </c>
-      <c r="K8" s="5"/>
-      <c r="L8" s="6" t="s">
-        <v>204</v>
-      </c>
+      <c r="K8" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="L8" s="5"/>
       <c r="M8" s="15" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="24">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="108">
       <c r="A9" s="5">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>137</v>
@@ -9951,19 +9944,19 @@
         <v>90</v>
       </c>
       <c r="D9" s="5">
-        <v>4.4000000000000004</v>
+        <v>4.3</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>1294</v>
-      </c>
-      <c r="H9" s="49" t="s">
-        <v>1281</v>
+        <v>1293</v>
+      </c>
+      <c r="H9" t="s">
+        <v>1263</v>
       </c>
       <c r="I9" s="6" t="s">
         <v>1231</v>
@@ -9971,36 +9964,38 @@
       <c r="J9" s="6" t="s">
         <v>1231</v>
       </c>
-      <c r="K9" s="6" t="s">
-        <v>230</v>
-      </c>
-      <c r="L9" s="9"/>
-      <c r="M9" s="15"/>
-    </row>
-    <row r="10" spans="1:14" ht="108">
+      <c r="K9" s="5"/>
+      <c r="L9" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="M9" s="15" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="36">
       <c r="A10" s="5">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>137</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="D10" s="5">
-        <v>12.1</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>1295</v>
-      </c>
-      <c r="H10" t="s">
-        <v>1264</v>
+        <v>98</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>1294</v>
+      </c>
+      <c r="H10" s="49" t="s">
+        <v>1281</v>
       </c>
       <c r="I10" s="6" t="s">
         <v>1231</v>
@@ -10011,14 +10006,12 @@
       <c r="K10" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="L10" s="5"/>
-      <c r="M10" s="15" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="24">
+      <c r="L10" s="9"/>
+      <c r="M10" s="15"/>
+    </row>
+    <row r="11" spans="1:14" ht="108">
       <c r="A11" s="5">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>137</v>
@@ -10027,19 +10020,19 @@
         <v>99</v>
       </c>
       <c r="D11" s="5">
-        <v>12.2</v>
+        <v>12.1</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="H11" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="I11" s="6" t="s">
         <v>1231</v>
@@ -10051,11 +10044,13 @@
         <v>230</v>
       </c>
       <c r="L11" s="5"/>
-      <c r="M11" s="15"/>
+      <c r="M11" s="15" t="s">
+        <v>332</v>
+      </c>
     </row>
     <row r="12" spans="1:14" ht="24">
       <c r="A12" s="5">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>137</v>
@@ -10064,19 +10059,19 @@
         <v>99</v>
       </c>
       <c r="D12" s="5">
-        <v>12.3</v>
+        <v>12.2</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="H12" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="I12" s="6" t="s">
         <v>1231</v>
@@ -10090,9 +10085,9 @@
       <c r="L12" s="5"/>
       <c r="M12" s="15"/>
     </row>
-    <row r="13" spans="1:14" ht="24" hidden="1">
+    <row r="13" spans="1:14" ht="36">
       <c r="A13" s="5">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>137</v>
@@ -10101,27 +10096,35 @@
         <v>99</v>
       </c>
       <c r="D13" s="5">
-        <v>12.4</v>
+        <v>12.3</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
+        <v>105</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>1297</v>
+      </c>
+      <c r="H13" t="s">
+        <v>1266</v>
+      </c>
       <c r="I13" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
+        <v>1231</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>1231</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>230</v>
+      </c>
       <c r="L13" s="5"/>
       <c r="M13" s="15"/>
     </row>
-    <row r="14" spans="1:14" ht="36">
+    <row r="14" spans="1:14" ht="24" hidden="1">
       <c r="A14" s="5">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>137</v>
@@ -10130,35 +10133,27 @@
         <v>99</v>
       </c>
       <c r="D14" s="5">
-        <v>12.5</v>
+        <v>12.4</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>1311</v>
-      </c>
-      <c r="H14" s="49" t="s">
-        <v>1273</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
       <c r="I14" s="6" t="s">
-        <v>1231</v>
-      </c>
-      <c r="J14" s="6" t="s">
-        <v>1231</v>
-      </c>
-      <c r="K14" s="6" t="s">
-        <v>230</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
       <c r="L14" s="5"/>
       <c r="M14" s="15"/>
     </row>
-    <row r="15" spans="1:14" ht="24">
+    <row r="15" spans="1:14" ht="36">
       <c r="A15" s="5">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>137</v>
@@ -10167,19 +10162,19 @@
         <v>99</v>
       </c>
       <c r="D15" s="5">
-        <v>12.6</v>
+        <v>12.5</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>1</v>
+        <v>108</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G15" s="56" t="s">
-        <v>1298</v>
+        <v>109</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>1311</v>
       </c>
       <c r="H15" s="49" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="I15" s="6" t="s">
         <v>1231</v>
@@ -10195,28 +10190,28 @@
     </row>
     <row r="16" spans="1:14" ht="36">
       <c r="A16" s="5">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>137</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="D16" s="5">
-        <v>13.1</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>111</v>
+        <v>12.6</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>1</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>112</v>
+        <v>5</v>
       </c>
       <c r="G16" s="56" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="H16" s="49" t="s">
-        <v>1267</v>
+        <v>1274</v>
       </c>
       <c r="I16" s="6" t="s">
         <v>1231</v>
@@ -10230,9 +10225,9 @@
       <c r="L16" s="5"/>
       <c r="M16" s="15"/>
     </row>
-    <row r="17" spans="1:13" ht="24">
+    <row r="17" spans="1:13" ht="36">
       <c r="A17" s="5">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>137</v>
@@ -10241,19 +10236,19 @@
         <v>110</v>
       </c>
       <c r="D17" s="5">
-        <v>13.2</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>113</v>
+        <v>13.1</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>111</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G17" s="56" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="H17" s="49" t="s">
-        <v>1277</v>
+        <v>1267</v>
       </c>
       <c r="I17" s="6" t="s">
         <v>1231</v>
@@ -10269,7 +10264,7 @@
     </row>
     <row r="18" spans="1:13" ht="24">
       <c r="A18" s="5">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>137</v>
@@ -10278,19 +10273,19 @@
         <v>110</v>
       </c>
       <c r="D18" s="5">
-        <v>13.3</v>
+        <v>13.2</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="G18" s="11" t="s">
-        <v>1301</v>
+        <v>114</v>
+      </c>
+      <c r="G18" s="56" t="s">
+        <v>1300</v>
       </c>
       <c r="H18" s="49" t="s">
-        <v>1275</v>
+        <v>1277</v>
       </c>
       <c r="I18" s="6" t="s">
         <v>1231</v>
@@ -10304,9 +10299,9 @@
       <c r="L18" s="5"/>
       <c r="M18" s="15"/>
     </row>
-    <row r="19" spans="1:13" ht="30">
+    <row r="19" spans="1:13" ht="24">
       <c r="A19" s="5">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>137</v>
@@ -10315,19 +10310,19 @@
         <v>110</v>
       </c>
       <c r="D19" s="5">
-        <v>13.4</v>
+        <v>13.3</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>1302</v>
-      </c>
-      <c r="H19" s="50" t="s">
-        <v>1276</v>
+        <v>116</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>1301</v>
+      </c>
+      <c r="H19" s="49" t="s">
+        <v>1275</v>
       </c>
       <c r="I19" s="6" t="s">
         <v>1231</v>
@@ -10341,30 +10336,30 @@
       <c r="L19" s="5"/>
       <c r="M19" s="15"/>
     </row>
-    <row r="20" spans="1:13" ht="24">
+    <row r="20" spans="1:13" ht="36">
       <c r="A20" s="5">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>137</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="D20" s="5">
-        <v>14.1</v>
+        <v>13.4</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>1303</v>
-      </c>
-      <c r="H20" s="49" t="s">
-        <v>1268</v>
+        <v>1302</v>
+      </c>
+      <c r="H20" s="50" t="s">
+        <v>1276</v>
       </c>
       <c r="I20" s="6" t="s">
         <v>1231</v>
@@ -10380,28 +10375,28 @@
     </row>
     <row r="21" spans="1:13" ht="24">
       <c r="A21" s="5">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>137</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D21" s="5">
-        <v>15.1</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>122</v>
+        <v>14.1</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>120</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
       <c r="H21" s="49" t="s">
-        <v>1279</v>
+        <v>1268</v>
       </c>
       <c r="I21" s="6" t="s">
         <v>1231</v>
@@ -10417,28 +10412,28 @@
     </row>
     <row r="22" spans="1:13" ht="24">
       <c r="A22" s="5">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>137</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D22" s="5">
-        <v>16.100000000000001</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>125</v>
+        <v>15.1</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>122</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>1310</v>
+        <v>1304</v>
       </c>
       <c r="H22" s="49" t="s">
-        <v>1278</v>
+        <v>1279</v>
       </c>
       <c r="I22" s="6" t="s">
         <v>1231</v>
@@ -10452,30 +10447,30 @@
       <c r="L22" s="5"/>
       <c r="M22" s="15"/>
     </row>
-    <row r="23" spans="1:13" ht="24">
+    <row r="23" spans="1:13" ht="36">
       <c r="A23" s="5">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>137</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D23" s="5">
-        <v>18.100000000000001</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>1305</v>
-      </c>
-      <c r="H23" t="s">
-        <v>1269</v>
+        <v>1310</v>
+      </c>
+      <c r="H23" s="49" t="s">
+        <v>1278</v>
       </c>
       <c r="I23" s="6" t="s">
         <v>1231</v>
@@ -10489,30 +10484,30 @@
       <c r="L23" s="5"/>
       <c r="M23" s="15"/>
     </row>
-    <row r="24" spans="1:13" ht="24">
+    <row r="24" spans="1:13" ht="36">
       <c r="A24" s="5">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>137</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D24" s="5">
-        <v>19.100000000000001</v>
+        <v>18.100000000000001</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>1306</v>
-      </c>
-      <c r="H24" s="49" t="s">
-        <v>1280</v>
+        <v>1305</v>
+      </c>
+      <c r="H24" t="s">
+        <v>1269</v>
       </c>
       <c r="I24" s="6" t="s">
         <v>1231</v>
@@ -10528,7 +10523,7 @@
     </row>
     <row r="25" spans="1:13" ht="24">
       <c r="A25" s="5">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>137</v>
@@ -10537,19 +10532,19 @@
         <v>129</v>
       </c>
       <c r="D25" s="5">
-        <v>19.2</v>
+        <v>19.100000000000001</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>1307</v>
-      </c>
-      <c r="H25" t="s">
-        <v>1270</v>
+        <v>1306</v>
+      </c>
+      <c r="H25" s="49" t="s">
+        <v>1280</v>
       </c>
       <c r="I25" s="6" t="s">
         <v>1231</v>
@@ -10565,28 +10560,28 @@
     </row>
     <row r="26" spans="1:13" ht="24">
       <c r="A26" s="5">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>137</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>751</v>
+        <v>129</v>
       </c>
       <c r="D26" s="5">
-        <v>21</v>
+        <v>19.2</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>750</v>
+        <v>132</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>752</v>
+        <v>133</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="H26" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="I26" s="6" t="s">
         <v>1231</v>
@@ -10600,30 +10595,30 @@
       <c r="L26" s="5"/>
       <c r="M26" s="15"/>
     </row>
-    <row r="27" spans="1:13" ht="24">
+    <row r="27" spans="1:13" ht="36">
       <c r="A27" s="5">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>137</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>1338</v>
+        <v>751</v>
       </c>
       <c r="D27" s="5">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>1338</v>
+        <v>750</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="G27" t="s">
-        <v>1349</v>
+        <v>752</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>1308</v>
       </c>
       <c r="H27" t="s">
-        <v>1339</v>
+        <v>1271</v>
       </c>
       <c r="I27" s="6" t="s">
         <v>1231</v>
@@ -10637,119 +10632,157 @@
       <c r="L27" s="5"/>
       <c r="M27" s="15"/>
     </row>
-    <row r="28" spans="1:13" ht="24" hidden="1">
+    <row r="28" spans="1:13" ht="24">
       <c r="A28" s="5">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="D28" s="5"/>
+        <v>1338</v>
+      </c>
+      <c r="D28" s="5">
+        <v>12</v>
+      </c>
       <c r="E28" s="5" t="s">
-        <v>139</v>
+        <v>1338</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5"/>
-      <c r="I28" s="5"/>
-      <c r="J28" s="5"/>
-      <c r="K28" s="5"/>
+        <v>107</v>
+      </c>
+      <c r="G28" t="s">
+        <v>1349</v>
+      </c>
+      <c r="H28" t="s">
+        <v>1339</v>
+      </c>
+      <c r="I28" s="6" t="s">
+        <v>1231</v>
+      </c>
+      <c r="J28" s="6" t="s">
+        <v>1231</v>
+      </c>
+      <c r="K28" s="6" t="s">
+        <v>230</v>
+      </c>
       <c r="L28" s="5"/>
       <c r="M28" s="15"/>
     </row>
-    <row r="29" spans="1:13" ht="36" hidden="1">
-      <c r="A29" s="17">
+    <row r="29" spans="1:13" ht="24" hidden="1">
+      <c r="A29" s="5">
+        <v>26</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="15"/>
+    </row>
+    <row r="30" spans="1:13" ht="48" hidden="1">
+      <c r="A30" s="17">
         <v>27</v>
       </c>
-      <c r="B29" s="17" t="s">
+      <c r="B30" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="C29" s="17" t="s">
+      <c r="C30" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="D29" s="17"/>
-      <c r="E29" s="17" t="s">
+      <c r="D30" s="17"/>
+      <c r="E30" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="F29" s="17" t="s">
+      <c r="F30" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="G29" s="17"/>
-      <c r="H29" s="17"/>
-      <c r="I29" s="17"/>
-      <c r="J29" s="17"/>
-      <c r="K29" s="17"/>
-      <c r="L29" s="17"/>
-      <c r="M29" s="18"/>
-    </row>
-    <row r="30" spans="1:13" ht="24">
-      <c r="A30" s="61">
-        <v>26</v>
-      </c>
-      <c r="B30" s="61" t="s">
+      <c r="G30" s="17"/>
+      <c r="H30" s="17"/>
+      <c r="I30" s="17"/>
+      <c r="J30" s="17"/>
+      <c r="K30" s="17"/>
+      <c r="L30" s="17"/>
+      <c r="M30" s="18"/>
+    </row>
+    <row r="31" spans="1:13" ht="24">
+      <c r="A31" s="61">
+        <v>25</v>
+      </c>
+      <c r="B31" s="61" t="s">
         <v>137</v>
       </c>
-      <c r="C30" s="61" t="s">
+      <c r="C31" s="61" t="s">
         <v>134</v>
       </c>
-      <c r="D30" s="61">
+      <c r="D31" s="61">
         <v>25.1</v>
       </c>
-      <c r="E30" s="61" t="s">
+      <c r="E31" s="61" t="s">
         <v>134</v>
       </c>
-      <c r="F30" s="61" t="s">
+      <c r="F31" s="61" t="s">
         <v>135</v>
       </c>
-      <c r="G30" s="62" t="s">
+      <c r="G31" s="62" t="s">
         <v>1309</v>
       </c>
-      <c r="H30" s="61" t="s">
+      <c r="H31" s="61" t="s">
         <v>1272</v>
       </c>
-      <c r="I30" s="61" t="s">
+      <c r="I31" s="61" t="s">
         <v>1231</v>
       </c>
-      <c r="J30" s="61" t="s">
+      <c r="J31" s="61" t="s">
         <v>1231</v>
       </c>
-      <c r="K30" s="63" t="s">
+      <c r="K31" s="63" t="s">
         <v>230</v>
       </c>
-      <c r="L30" s="61"/>
-      <c r="M30" s="64"/>
+      <c r="L31" s="61"/>
+      <c r="M31" s="64"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H14" r:id="rId1"/>
-    <hyperlink ref="H15" r:id="rId2"/>
-    <hyperlink ref="H18" r:id="rId3"/>
-    <hyperlink ref="H19" r:id="rId4"/>
-    <hyperlink ref="H16" r:id="rId5"/>
-    <hyperlink ref="H17" r:id="rId6"/>
-    <hyperlink ref="H20" r:id="rId7"/>
-    <hyperlink ref="H22" r:id="rId8"/>
-    <hyperlink ref="H21" r:id="rId9"/>
-    <hyperlink ref="H24" r:id="rId10"/>
-    <hyperlink ref="H9" r:id="rId11"/>
-    <hyperlink ref="H6" r:id="rId12"/>
+    <hyperlink ref="H15" r:id="rId1"/>
+    <hyperlink ref="H16" r:id="rId2"/>
+    <hyperlink ref="H19" r:id="rId3"/>
+    <hyperlink ref="H20" r:id="rId4"/>
+    <hyperlink ref="H17" r:id="rId5"/>
+    <hyperlink ref="H18" r:id="rId6"/>
+    <hyperlink ref="H21" r:id="rId7"/>
+    <hyperlink ref="H23" r:id="rId8"/>
+    <hyperlink ref="H22" r:id="rId9"/>
+    <hyperlink ref="H25" r:id="rId10"/>
+    <hyperlink ref="H10" r:id="rId11"/>
+    <hyperlink ref="H7" r:id="rId12"/>
     <hyperlink ref="H2" r:id="rId13"/>
     <hyperlink ref="G2" r:id="rId14"/>
-    <hyperlink ref="G6" r:id="rId15"/>
-    <hyperlink ref="G15" r:id="rId16"/>
-    <hyperlink ref="G16" r:id="rId17"/>
-    <hyperlink ref="G17" r:id="rId18"/>
-    <hyperlink ref="G30" r:id="rId19"/>
+    <hyperlink ref="G7" r:id="rId15"/>
+    <hyperlink ref="G16" r:id="rId16"/>
+    <hyperlink ref="G17" r:id="rId17"/>
+    <hyperlink ref="G18" r:id="rId18"/>
+    <hyperlink ref="G31" r:id="rId19"/>
+    <hyperlink ref="H4" r:id="rId20"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId20"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId21"/>
   <tableParts count="1">
-    <tablePart r:id="rId21"/>
+    <tablePart r:id="rId22"/>
   </tableParts>
 </worksheet>
 </file>
@@ -12953,7 +12986,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G27" sqref="G27"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13010,7 +13043,7 @@
         <v>1249</v>
       </c>
     </row>
-    <row r="2" spans="1:12" hidden="1">
+    <row r="2" spans="1:12">
       <c r="A2" s="19">
         <v>1</v>
       </c>
@@ -13038,7 +13071,7 @@
       <c r="K2" s="53"/>
       <c r="L2" s="52"/>
     </row>
-    <row r="3" spans="1:12" ht="24" hidden="1">
+    <row r="3" spans="1:12" ht="24">
       <c r="A3" s="19">
         <v>2</v>
       </c>
@@ -13064,7 +13097,7 @@
       <c r="K3" s="15"/>
       <c r="L3" s="45"/>
     </row>
-    <row r="4" spans="1:12" ht="24" hidden="1">
+    <row r="4" spans="1:12" ht="24">
       <c r="A4" s="19">
         <v>3</v>
       </c>
@@ -13090,7 +13123,7 @@
       <c r="K4" s="15"/>
       <c r="L4" s="6"/>
     </row>
-    <row r="5" spans="1:12" hidden="1">
+    <row r="5" spans="1:12">
       <c r="A5" s="19">
         <v>4</v>
       </c>
@@ -13118,7 +13151,7 @@
       <c r="K5" s="15"/>
       <c r="L5" s="6"/>
     </row>
-    <row r="6" spans="1:12" hidden="1">
+    <row r="6" spans="1:12">
       <c r="A6" s="19">
         <v>5</v>
       </c>
@@ -13144,7 +13177,7 @@
       <c r="K6" s="15"/>
       <c r="L6" s="6"/>
     </row>
-    <row r="7" spans="1:12" hidden="1">
+    <row r="7" spans="1:12">
       <c r="A7" s="19">
         <v>6</v>
       </c>
@@ -13172,7 +13205,7 @@
       <c r="K7" s="15"/>
       <c r="L7" s="6"/>
     </row>
-    <row r="8" spans="1:12" hidden="1">
+    <row r="8" spans="1:12">
       <c r="A8" s="19">
         <v>7</v>
       </c>
@@ -13202,7 +13235,7 @@
       <c r="K8" s="15"/>
       <c r="L8" s="6"/>
     </row>
-    <row r="9" spans="1:12" hidden="1">
+    <row r="9" spans="1:12">
       <c r="A9" s="19">
         <v>8</v>
       </c>
@@ -13232,7 +13265,7 @@
       <c r="K9" s="15"/>
       <c r="L9" s="6"/>
     </row>
-    <row r="10" spans="1:12" hidden="1">
+    <row r="10" spans="1:12">
       <c r="A10" s="19">
         <v>9</v>
       </c>
@@ -13264,7 +13297,7 @@
       </c>
       <c r="L10" s="6"/>
     </row>
-    <row r="11" spans="1:12" hidden="1">
+    <row r="11" spans="1:12">
       <c r="A11" s="19">
         <v>10</v>
       </c>
@@ -13292,7 +13325,7 @@
       <c r="K11" s="15"/>
       <c r="L11" s="6"/>
     </row>
-    <row r="12" spans="1:12" hidden="1">
+    <row r="12" spans="1:12">
       <c r="A12" s="19">
         <v>11</v>
       </c>
@@ -13320,7 +13353,7 @@
       <c r="K12" s="15"/>
       <c r="L12" s="6"/>
     </row>
-    <row r="13" spans="1:12" hidden="1">
+    <row r="13" spans="1:12">
       <c r="A13" s="19">
         <v>12</v>
       </c>
@@ -13350,7 +13383,7 @@
       <c r="K13" s="15"/>
       <c r="L13" s="6"/>
     </row>
-    <row r="14" spans="1:12" hidden="1">
+    <row r="14" spans="1:12">
       <c r="A14" s="19">
         <v>13</v>
       </c>
@@ -13378,7 +13411,7 @@
       <c r="K14" s="15"/>
       <c r="L14" s="6"/>
     </row>
-    <row r="15" spans="1:12" hidden="1">
+    <row r="15" spans="1:12">
       <c r="A15" s="19">
         <v>14</v>
       </c>
@@ -13404,7 +13437,7 @@
       <c r="K15" s="15"/>
       <c r="L15" s="6"/>
     </row>
-    <row r="16" spans="1:12" hidden="1">
+    <row r="16" spans="1:12">
       <c r="A16" s="19">
         <v>15</v>
       </c>
@@ -13430,7 +13463,7 @@
       <c r="K16" s="15"/>
       <c r="L16" s="6"/>
     </row>
-    <row r="17" spans="1:12" ht="24" hidden="1">
+    <row r="17" spans="1:12" ht="24">
       <c r="A17" s="19">
         <v>16</v>
       </c>
@@ -13456,7 +13489,7 @@
       <c r="K17" s="15"/>
       <c r="L17" s="6"/>
     </row>
-    <row r="18" spans="1:12" hidden="1">
+    <row r="18" spans="1:12">
       <c r="A18" s="19">
         <v>17</v>
       </c>
@@ -13484,7 +13517,7 @@
       <c r="K18" s="15"/>
       <c r="L18" s="6"/>
     </row>
-    <row r="19" spans="1:12" hidden="1">
+    <row r="19" spans="1:12">
       <c r="A19" s="19">
         <v>18</v>
       </c>
@@ -13512,7 +13545,7 @@
       <c r="K19" s="15"/>
       <c r="L19" s="6"/>
     </row>
-    <row r="20" spans="1:12" ht="24" hidden="1">
+    <row r="20" spans="1:12">
       <c r="A20" s="19">
         <v>19</v>
       </c>
@@ -13540,7 +13573,7 @@
       <c r="K20" s="15"/>
       <c r="L20" s="6"/>
     </row>
-    <row r="21" spans="1:12" ht="24" hidden="1">
+    <row r="21" spans="1:12" ht="24">
       <c r="A21" s="19">
         <v>20</v>
       </c>
@@ -13568,7 +13601,7 @@
       <c r="K21" s="15"/>
       <c r="L21" s="6"/>
     </row>
-    <row r="22" spans="1:12" ht="24" hidden="1">
+    <row r="22" spans="1:12" ht="24">
       <c r="A22" s="19">
         <v>21</v>
       </c>
@@ -13596,7 +13629,7 @@
       <c r="K22" s="15"/>
       <c r="L22" s="6"/>
     </row>
-    <row r="23" spans="1:12" ht="24" hidden="1">
+    <row r="23" spans="1:12" ht="24">
       <c r="A23" s="19">
         <v>22</v>
       </c>
@@ -13624,7 +13657,7 @@
       <c r="K23" s="15"/>
       <c r="L23" s="6"/>
     </row>
-    <row r="24" spans="1:12" hidden="1">
+    <row r="24" spans="1:12">
       <c r="A24" s="19">
         <v>23</v>
       </c>
@@ -13652,7 +13685,7 @@
       <c r="K24" s="15"/>
       <c r="L24" s="6"/>
     </row>
-    <row r="25" spans="1:12" hidden="1">
+    <row r="25" spans="1:12">
       <c r="A25" s="19">
         <v>24</v>
       </c>
@@ -13680,7 +13713,7 @@
       <c r="K25" s="15"/>
       <c r="L25" s="6"/>
     </row>
-    <row r="26" spans="1:12" hidden="1">
+    <row r="26" spans="1:12">
       <c r="A26" s="19">
         <v>25</v>
       </c>
@@ -13736,7 +13769,7 @@
       <c r="K27" s="15"/>
       <c r="L27" s="6"/>
     </row>
-    <row r="28" spans="1:12" ht="24" hidden="1">
+    <row r="28" spans="1:12" ht="24">
       <c r="A28" s="19">
         <v>27</v>
       </c>
@@ -13764,7 +13797,7 @@
       <c r="K28" s="15"/>
       <c r="L28" s="6"/>
     </row>
-    <row r="29" spans="1:12" ht="24" hidden="1">
+    <row r="29" spans="1:12" ht="24">
       <c r="A29" s="19">
         <v>28</v>
       </c>
@@ -13792,7 +13825,7 @@
       <c r="K29" s="15"/>
       <c r="L29" s="6"/>
     </row>
-    <row r="30" spans="1:12" ht="24" hidden="1">
+    <row r="30" spans="1:12" ht="24">
       <c r="A30" s="19">
         <v>29</v>
       </c>
@@ -13824,7 +13857,7 @@
         <v>1240</v>
       </c>
     </row>
-    <row r="31" spans="1:12" hidden="1">
+    <row r="31" spans="1:12">
       <c r="A31" s="19">
         <v>30</v>
       </c>
@@ -13856,7 +13889,7 @@
         <v>1241</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="24" hidden="1">
+    <row r="32" spans="1:12" ht="24">
       <c r="A32" s="19">
         <v>31</v>
       </c>
@@ -13888,7 +13921,7 @@
         <v>1242</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="36" hidden="1">
+    <row r="33" spans="1:12" ht="36">
       <c r="A33" s="19">
         <v>32</v>
       </c>
@@ -13920,7 +13953,7 @@
         <v>1247</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="48" hidden="1">
+    <row r="34" spans="1:12" ht="48">
       <c r="A34" s="19">
         <v>33</v>
       </c>
@@ -13952,7 +13985,7 @@
         <v>1243</v>
       </c>
     </row>
-    <row r="35" spans="1:12" hidden="1">
+    <row r="35" spans="1:12">
       <c r="A35" s="19">
         <v>34</v>
       </c>
@@ -13986,7 +14019,7 @@
         <v>1248</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="24" hidden="1">
+    <row r="36" spans="1:12" ht="24">
       <c r="A36" s="19">
         <v>35</v>
       </c>
@@ -14018,7 +14051,7 @@
         <v>1244</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="24" hidden="1">
+    <row r="37" spans="1:12" ht="24">
       <c r="A37" s="19">
         <v>36</v>
       </c>
@@ -14050,7 +14083,7 @@
         <v>1240</v>
       </c>
     </row>
-    <row r="38" spans="1:12" hidden="1">
+    <row r="38" spans="1:12">
       <c r="A38" s="19">
         <v>37</v>
       </c>
@@ -14082,7 +14115,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:12" hidden="1">
+    <row r="39" spans="1:12">
       <c r="A39" s="19">
         <v>38</v>
       </c>
@@ -14112,7 +14145,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:12" hidden="1">
+    <row r="40" spans="1:12">
       <c r="A40" s="19">
         <v>39</v>
       </c>
@@ -14142,7 +14175,7 @@
         <v>892</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="24" hidden="1">
+    <row r="41" spans="1:12" ht="24">
       <c r="A41" s="19">
         <v>40</v>
       </c>
@@ -14172,7 +14205,7 @@
         <v>1245</v>
       </c>
     </row>
-    <row r="42" spans="1:12" hidden="1">
+    <row r="42" spans="1:12">
       <c r="A42" s="19">
         <v>41</v>
       </c>
@@ -14202,7 +14235,7 @@
         <v>1246</v>
       </c>
     </row>
-    <row r="43" spans="1:12" hidden="1">
+    <row r="43" spans="1:12">
       <c r="A43" s="19">
         <v>42</v>
       </c>
@@ -14232,7 +14265,7 @@
         <v>1246</v>
       </c>
     </row>
-    <row r="44" spans="1:12" hidden="1">
+    <row r="44" spans="1:12">
       <c r="A44" s="19">
         <v>43</v>
       </c>
@@ -14266,7 +14299,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="45" spans="1:12" hidden="1">
+    <row r="45" spans="1:12">
       <c r="A45" s="19">
         <v>44</v>
       </c>
@@ -14296,7 +14329,7 @@
         <v>1014</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="24" hidden="1">
+    <row r="46" spans="1:12" ht="24">
       <c r="A46" s="19">
         <v>45</v>
       </c>
@@ -14330,7 +14363,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="24" hidden="1">
+    <row r="47" spans="1:12" ht="24">
       <c r="A47" s="19">
         <v>46</v>
       </c>
@@ -14364,7 +14397,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="48" spans="1:12" hidden="1">
+    <row r="48" spans="1:12">
       <c r="A48" s="19">
         <v>47</v>
       </c>
@@ -14394,7 +14427,7 @@
         <v>1246</v>
       </c>
     </row>
-    <row r="49" spans="1:16" ht="24" hidden="1">
+    <row r="49" spans="1:16" ht="24">
       <c r="A49" s="19">
         <v>48</v>
       </c>
@@ -14424,7 +14457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:16" hidden="1">
+    <row r="50" spans="1:16">
       <c r="A50" s="19">
         <v>49</v>
       </c>
@@ -14454,7 +14487,7 @@
         <v>1246</v>
       </c>
     </row>
-    <row r="51" spans="1:16" hidden="1">
+    <row r="51" spans="1:16">
       <c r="A51" s="19">
         <v>50</v>
       </c>
@@ -14484,7 +14517,7 @@
         <v>1246</v>
       </c>
     </row>
-    <row r="52" spans="1:16" ht="24" hidden="1">
+    <row r="52" spans="1:16" ht="24">
       <c r="A52" s="19">
         <v>51</v>
       </c>
@@ -14518,7 +14551,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="53" spans="1:16" hidden="1">
+    <row r="53" spans="1:16">
       <c r="A53" s="19">
         <v>52</v>
       </c>
@@ -14546,7 +14579,7 @@
       <c r="K53" s="15"/>
       <c r="L53" s="6"/>
     </row>
-    <row r="54" spans="1:16" hidden="1">
+    <row r="54" spans="1:16">
       <c r="A54" s="19">
         <v>53</v>
       </c>
@@ -14574,7 +14607,7 @@
       <c r="K54" s="15"/>
       <c r="L54" s="6"/>
     </row>
-    <row r="55" spans="1:16" hidden="1">
+    <row r="55" spans="1:16">
       <c r="A55" s="19">
         <v>54</v>
       </c>
@@ -14602,7 +14635,7 @@
       <c r="K55" s="15"/>
       <c r="L55" s="6"/>
     </row>
-    <row r="56" spans="1:16" hidden="1">
+    <row r="56" spans="1:16">
       <c r="A56" s="19">
         <v>55</v>
       </c>
@@ -14630,7 +14663,7 @@
       <c r="K56" s="15"/>
       <c r="L56" s="6"/>
     </row>
-    <row r="57" spans="1:16" hidden="1">
+    <row r="57" spans="1:16">
       <c r="A57" s="19">
         <v>56</v>
       </c>
@@ -14660,7 +14693,7 @@
       <c r="K57" s="15"/>
       <c r="L57" s="6"/>
     </row>
-    <row r="58" spans="1:16" hidden="1">
+    <row r="58" spans="1:16">
       <c r="A58" s="19">
         <v>57</v>
       </c>
@@ -14688,7 +14721,7 @@
       <c r="K58" s="15"/>
       <c r="L58" s="6"/>
     </row>
-    <row r="59" spans="1:16" hidden="1">
+    <row r="59" spans="1:16">
       <c r="A59" s="19">
         <v>58</v>
       </c>
@@ -14716,7 +14749,7 @@
       <c r="K59" s="15"/>
       <c r="L59" s="6"/>
     </row>
-    <row r="60" spans="1:16" hidden="1">
+    <row r="60" spans="1:16">
       <c r="A60" s="19">
         <v>59</v>
       </c>
@@ -14752,7 +14785,7 @@
         <v>79.599999999999994</v>
       </c>
     </row>
-    <row r="61" spans="1:16" hidden="1">
+    <row r="61" spans="1:16">
       <c r="A61" s="19">
         <v>60</v>
       </c>
@@ -14780,7 +14813,7 @@
       <c r="K61" s="15"/>
       <c r="L61" s="6"/>
     </row>
-    <row r="62" spans="1:16" hidden="1">
+    <row r="62" spans="1:16">
       <c r="A62" s="19">
         <v>61</v>
       </c>
@@ -14808,7 +14841,7 @@
       <c r="K62" s="15"/>
       <c r="L62" s="6"/>
     </row>
-    <row r="63" spans="1:16" hidden="1">
+    <row r="63" spans="1:16">
       <c r="A63" s="19">
         <v>62</v>
       </c>
@@ -14836,7 +14869,7 @@
       <c r="K63" s="15"/>
       <c r="L63" s="6"/>
     </row>
-    <row r="64" spans="1:16" hidden="1">
+    <row r="64" spans="1:16">
       <c r="A64" s="19">
         <v>63</v>
       </c>
@@ -14864,7 +14897,7 @@
       <c r="K64" s="15"/>
       <c r="L64" s="6"/>
     </row>
-    <row r="65" spans="1:12" hidden="1">
+    <row r="65" spans="1:12">
       <c r="A65" s="19">
         <v>64</v>
       </c>
@@ -14892,7 +14925,7 @@
       <c r="K65" s="15"/>
       <c r="L65" s="6"/>
     </row>
-    <row r="66" spans="1:12" hidden="1">
+    <row r="66" spans="1:12">
       <c r="A66" s="19">
         <v>65</v>
       </c>
@@ -14920,7 +14953,7 @@
       <c r="K66" s="15"/>
       <c r="L66" s="6"/>
     </row>
-    <row r="67" spans="1:12" hidden="1">
+    <row r="67" spans="1:12">
       <c r="A67" s="19">
         <v>66</v>
       </c>
@@ -14948,7 +14981,7 @@
       <c r="K67" s="15"/>
       <c r="L67" s="6"/>
     </row>
-    <row r="68" spans="1:12" hidden="1">
+    <row r="68" spans="1:12">
       <c r="A68" s="19">
         <v>67</v>
       </c>
@@ -14976,7 +15009,7 @@
       <c r="K68" s="15"/>
       <c r="L68" s="6"/>
     </row>
-    <row r="69" spans="1:12" hidden="1">
+    <row r="69" spans="1:12">
       <c r="A69" s="19">
         <v>68</v>
       </c>
@@ -15004,7 +15037,7 @@
       <c r="K69" s="15"/>
       <c r="L69" s="6"/>
     </row>
-    <row r="70" spans="1:12" hidden="1">
+    <row r="70" spans="1:12">
       <c r="A70" s="19">
         <v>69</v>
       </c>
@@ -15032,7 +15065,7 @@
       <c r="K70" s="15"/>
       <c r="L70" s="6"/>
     </row>
-    <row r="71" spans="1:12" hidden="1">
+    <row r="71" spans="1:12">
       <c r="A71" s="19">
         <v>70</v>
       </c>
@@ -15060,7 +15093,7 @@
       <c r="K71" s="15"/>
       <c r="L71" s="6"/>
     </row>
-    <row r="72" spans="1:12" ht="24" hidden="1">
+    <row r="72" spans="1:12" ht="24">
       <c r="A72" s="19">
         <v>71</v>
       </c>
@@ -15088,7 +15121,7 @@
       <c r="K72" s="15"/>
       <c r="L72" s="6"/>
     </row>
-    <row r="73" spans="1:12" hidden="1">
+    <row r="73" spans="1:12">
       <c r="A73" s="19">
         <v>72</v>
       </c>
@@ -15116,7 +15149,7 @@
       <c r="K73" s="15"/>
       <c r="L73" s="6"/>
     </row>
-    <row r="74" spans="1:12" hidden="1">
+    <row r="74" spans="1:12">
       <c r="A74" s="19">
         <v>73</v>
       </c>
@@ -15142,7 +15175,7 @@
       <c r="K74" s="15"/>
       <c r="L74" s="6"/>
     </row>
-    <row r="75" spans="1:12" hidden="1">
+    <row r="75" spans="1:12">
       <c r="A75" s="19">
         <v>74</v>
       </c>
@@ -15170,7 +15203,7 @@
       <c r="K75" s="15"/>
       <c r="L75" s="6"/>
     </row>
-    <row r="76" spans="1:12" hidden="1">
+    <row r="76" spans="1:12">
       <c r="A76" s="19">
         <v>75</v>
       </c>
@@ -15198,7 +15231,7 @@
       <c r="K76" s="15"/>
       <c r="L76" s="6"/>
     </row>
-    <row r="77" spans="1:12" hidden="1">
+    <row r="77" spans="1:12">
       <c r="A77" s="19">
         <v>76</v>
       </c>
@@ -15226,7 +15259,7 @@
       <c r="K77" s="15"/>
       <c r="L77" s="6"/>
     </row>
-    <row r="78" spans="1:12" hidden="1">
+    <row r="78" spans="1:12">
       <c r="A78" s="19">
         <v>77</v>
       </c>
@@ -15254,7 +15287,7 @@
       <c r="K78" s="15"/>
       <c r="L78" s="6"/>
     </row>
-    <row r="79" spans="1:12" hidden="1">
+    <row r="79" spans="1:12">
       <c r="A79" s="19">
         <v>78</v>
       </c>
@@ -15282,7 +15315,7 @@
       <c r="K79" s="15"/>
       <c r="L79" s="6"/>
     </row>
-    <row r="80" spans="1:12" hidden="1">
+    <row r="80" spans="1:12">
       <c r="A80" s="19">
         <v>79</v>
       </c>
@@ -15310,7 +15343,7 @@
       <c r="K80" s="15"/>
       <c r="L80" s="6"/>
     </row>
-    <row r="81" spans="1:12" hidden="1">
+    <row r="81" spans="1:12">
       <c r="A81" s="19">
         <v>80</v>
       </c>
@@ -15338,7 +15371,7 @@
       <c r="K81" s="15"/>
       <c r="L81" s="6"/>
     </row>
-    <row r="82" spans="1:12" hidden="1">
+    <row r="82" spans="1:12">
       <c r="A82" s="19">
         <v>81</v>
       </c>
@@ -15366,7 +15399,7 @@
       <c r="K82" s="15"/>
       <c r="L82" s="6"/>
     </row>
-    <row r="83" spans="1:12" hidden="1">
+    <row r="83" spans="1:12">
       <c r="A83" s="19">
         <v>82</v>
       </c>
@@ -15394,7 +15427,7 @@
       <c r="K83" s="15"/>
       <c r="L83" s="6"/>
     </row>
-    <row r="84" spans="1:12" hidden="1">
+    <row r="84" spans="1:12">
       <c r="A84" s="19">
         <v>83</v>
       </c>
@@ -15422,7 +15455,7 @@
       <c r="K84" s="15"/>
       <c r="L84" s="6"/>
     </row>
-    <row r="85" spans="1:12" hidden="1">
+    <row r="85" spans="1:12">
       <c r="A85" s="19">
         <v>84</v>
       </c>
@@ -15450,7 +15483,7 @@
       <c r="K85" s="15"/>
       <c r="L85" s="6"/>
     </row>
-    <row r="86" spans="1:12" hidden="1">
+    <row r="86" spans="1:12">
       <c r="A86" s="19">
         <v>85</v>
       </c>
@@ -15478,7 +15511,7 @@
       <c r="K86" s="15"/>
       <c r="L86" s="6"/>
     </row>
-    <row r="87" spans="1:12" hidden="1">
+    <row r="87" spans="1:12">
       <c r="A87" s="19">
         <v>86</v>
       </c>
@@ -15506,7 +15539,7 @@
       <c r="K87" s="15"/>
       <c r="L87" s="6"/>
     </row>
-    <row r="88" spans="1:12" hidden="1">
+    <row r="88" spans="1:12">
       <c r="A88" s="19">
         <v>87</v>
       </c>
@@ -15534,7 +15567,7 @@
       <c r="K88" s="15"/>
       <c r="L88" s="6"/>
     </row>
-    <row r="89" spans="1:12" hidden="1">
+    <row r="89" spans="1:12">
       <c r="A89" s="19">
         <v>88</v>
       </c>
@@ -15562,7 +15595,7 @@
       <c r="K89" s="15"/>
       <c r="L89" s="6"/>
     </row>
-    <row r="90" spans="1:12" hidden="1">
+    <row r="90" spans="1:12">
       <c r="A90" s="19">
         <v>89</v>
       </c>
@@ -15590,7 +15623,7 @@
       <c r="K90" s="15"/>
       <c r="L90" s="6"/>
     </row>
-    <row r="91" spans="1:12" ht="36" hidden="1">
+    <row r="91" spans="1:12" ht="36">
       <c r="A91" s="19">
         <v>90</v>
       </c>
@@ -15620,7 +15653,7 @@
       <c r="K91" s="15"/>
       <c r="L91" s="6"/>
     </row>
-    <row r="92" spans="1:12" hidden="1">
+    <row r="92" spans="1:12">
       <c r="A92" s="19">
         <v>91</v>
       </c>
@@ -15648,7 +15681,7 @@
       <c r="K92" s="15"/>
       <c r="L92" s="6"/>
     </row>
-    <row r="93" spans="1:12" hidden="1">
+    <row r="93" spans="1:12">
       <c r="A93" s="19">
         <v>92</v>
       </c>
@@ -15676,7 +15709,7 @@
       <c r="K93" s="15"/>
       <c r="L93" s="6"/>
     </row>
-    <row r="94" spans="1:12" hidden="1">
+    <row r="94" spans="1:12">
       <c r="A94" s="19">
         <v>93</v>
       </c>
@@ -15704,7 +15737,7 @@
       <c r="K94" s="15"/>
       <c r="L94" s="6"/>
     </row>
-    <row r="95" spans="1:12" hidden="1">
+    <row r="95" spans="1:12">
       <c r="A95" s="19">
         <v>94</v>
       </c>
@@ -15732,7 +15765,7 @@
       <c r="K95" s="15"/>
       <c r="L95" s="6"/>
     </row>
-    <row r="96" spans="1:12" hidden="1">
+    <row r="96" spans="1:12">
       <c r="A96" s="19">
         <v>95</v>
       </c>
@@ -15760,7 +15793,7 @@
       <c r="K96" s="15"/>
       <c r="L96" s="6"/>
     </row>
-    <row r="97" spans="1:12" hidden="1">
+    <row r="97" spans="1:12">
       <c r="A97" s="19">
         <v>96</v>
       </c>
@@ -15788,7 +15821,7 @@
       <c r="K97" s="15"/>
       <c r="L97" s="6"/>
     </row>
-    <row r="98" spans="1:12" hidden="1">
+    <row r="98" spans="1:12">
       <c r="A98" s="19">
         <v>97</v>
       </c>
@@ -15816,7 +15849,7 @@
       <c r="K98" s="15"/>
       <c r="L98" s="6"/>
     </row>
-    <row r="99" spans="1:12" hidden="1">
+    <row r="99" spans="1:12">
       <c r="A99" s="19">
         <v>98</v>
       </c>
@@ -15844,7 +15877,7 @@
       <c r="K99" s="15"/>
       <c r="L99" s="6"/>
     </row>
-    <row r="100" spans="1:12" hidden="1">
+    <row r="100" spans="1:12">
       <c r="A100" s="19">
         <v>99</v>
       </c>
@@ -15872,7 +15905,7 @@
       <c r="K100" s="15"/>
       <c r="L100" s="6"/>
     </row>
-    <row r="101" spans="1:12" hidden="1">
+    <row r="101" spans="1:12">
       <c r="A101" s="19">
         <v>100</v>
       </c>
@@ -15900,7 +15933,7 @@
       <c r="K101" s="15"/>
       <c r="L101" s="6"/>
     </row>
-    <row r="102" spans="1:12" hidden="1">
+    <row r="102" spans="1:12">
       <c r="A102" s="19">
         <v>101</v>
       </c>
@@ -15926,7 +15959,7 @@
       <c r="K102" s="15"/>
       <c r="L102" s="23"/>
     </row>
-    <row r="103" spans="1:12" hidden="1">
+    <row r="103" spans="1:12">
       <c r="A103" s="19">
         <v>102</v>
       </c>
@@ -15952,7 +15985,7 @@
       <c r="K103" s="15"/>
       <c r="L103" s="23"/>
     </row>
-    <row r="104" spans="1:12" hidden="1">
+    <row r="104" spans="1:12">
       <c r="A104" s="19">
         <v>103</v>
       </c>
@@ -15978,7 +16011,7 @@
       <c r="K104" s="15"/>
       <c r="L104" s="23"/>
     </row>
-    <row r="105" spans="1:12" hidden="1">
+    <row r="105" spans="1:12">
       <c r="A105" s="19">
         <v>104</v>
       </c>
@@ -16004,7 +16037,7 @@
       <c r="K105" s="15"/>
       <c r="L105" s="23"/>
     </row>
-    <row r="106" spans="1:12" ht="24" hidden="1">
+    <row r="106" spans="1:12" ht="24">
       <c r="A106" s="19">
         <v>105</v>
       </c>
@@ -16030,7 +16063,7 @@
       <c r="K106" s="15"/>
       <c r="L106" s="23"/>
     </row>
-    <row r="107" spans="1:12" hidden="1">
+    <row r="107" spans="1:12">
       <c r="A107" s="66">
         <v>101</v>
       </c>

</xml_diff>

<commit_message>
Upto All bug fix
</commit_message>
<xml_diff>
--- a/api_handler_app/Habile_Investak_API_Dictionary.xlsx
+++ b/api_handler_app/Habile_Investak_API_Dictionary.xlsx
@@ -8241,7 +8241,11 @@
     </filterColumn>
     <filterColumn colId="13"/>
     <filterColumn colId="14"/>
-    <filterColumn colId="15"/>
+    <filterColumn colId="15">
+      <filters>
+        <filter val="No"/>
+      </filters>
+    </filterColumn>
   </autoFilter>
   <tableColumns count="16">
     <tableColumn id="1" name="#" dataDxfId="89"/>
@@ -8671,7 +8675,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -9967,7 +9971,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomRight" activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10126,9 +10130,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1"/>
-    <hyperlink ref="L3:L4" r:id="rId2" display="http://nestuat.tradesmartonline.in/"/>
-    <hyperlink ref="K2" r:id="rId3"/>
+    <hyperlink ref="L3:L4" r:id="rId1" display="http://nestuat.tradesmartonline.in/"/>
+    <hyperlink ref="K2" r:id="rId2"/>
+    <hyperlink ref="L2" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
@@ -10146,7 +10150,7 @@
       <pane xSplit="5" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O2" sqref="O2"/>
+      <selection pane="bottomRight" activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10217,7 +10221,7 @@
         <v>1298</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="180">
+    <row r="2" spans="1:16" ht="180" hidden="1">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -10349,7 +10353,7 @@
         <v>1219</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="24">
+    <row r="5" spans="1:16" ht="24" hidden="1">
       <c r="A5" s="5">
         <v>3</v>
       </c>
@@ -10435,7 +10439,7 @@
       <c r="O6" s="5"/>
       <c r="P6" s="5"/>
     </row>
-    <row r="7" spans="1:16" ht="96">
+    <row r="7" spans="1:16" ht="96" hidden="1">
       <c r="A7" s="5">
         <v>4</v>
       </c>
@@ -10483,7 +10487,7 @@
         <v>1219</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="60">
+    <row r="8" spans="1:16" ht="60" hidden="1">
       <c r="A8" s="5">
         <v>5</v>
       </c>
@@ -10531,7 +10535,7 @@
         <v>1219</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="192">
+    <row r="9" spans="1:16" ht="192" hidden="1">
       <c r="A9" s="5">
         <v>6</v>
       </c>
@@ -10579,7 +10583,7 @@
         <v>1219</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="36">
+    <row r="10" spans="1:16" ht="36" hidden="1">
       <c r="A10" s="5">
         <v>7</v>
       </c>
@@ -10625,7 +10629,7 @@
         <v>1219</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="216">
+    <row r="11" spans="1:16" ht="216" hidden="1">
       <c r="A11" s="5">
         <v>8</v>
       </c>
@@ -10673,7 +10677,7 @@
         <v>1219</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="24">
+    <row r="12" spans="1:16" ht="24" hidden="1">
       <c r="A12" s="5">
         <v>9</v>
       </c>
@@ -10719,7 +10723,7 @@
         <v>1219</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="36">
+    <row r="13" spans="1:16" ht="36" hidden="1">
       <c r="A13" s="5">
         <v>10</v>
       </c>
@@ -10797,7 +10801,7 @@
       <c r="O14" s="5"/>
       <c r="P14" s="5"/>
     </row>
-    <row r="15" spans="1:16" ht="36">
+    <row r="15" spans="1:16" ht="36" hidden="1">
       <c r="A15" s="5">
         <v>11</v>
       </c>
@@ -10843,7 +10847,7 @@
         <v>1219</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="36">
+    <row r="16" spans="1:16" ht="36" hidden="1">
       <c r="A16" s="5">
         <v>12</v>
       </c>
@@ -10935,7 +10939,7 @@
         <v>1219</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="24">
+    <row r="18" spans="1:16" ht="24" hidden="1">
       <c r="A18" s="5">
         <v>14</v>
       </c>
@@ -10981,7 +10985,7 @@
         <v>1219</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="24">
+    <row r="19" spans="1:16" ht="24" hidden="1">
       <c r="A19" s="5">
         <v>15</v>
       </c>
@@ -11119,7 +11123,7 @@
         <v>1219</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="24">
+    <row r="22" spans="1:16" ht="24" hidden="1">
       <c r="A22" s="5">
         <v>18</v>
       </c>
@@ -11211,7 +11215,7 @@
         <v>1219</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="36">
+    <row r="24" spans="1:16" ht="36" hidden="1">
       <c r="A24" s="5">
         <v>20</v>
       </c>
@@ -11257,7 +11261,7 @@
         <v>1219</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="24">
+    <row r="25" spans="1:16" ht="24" hidden="1">
       <c r="A25" s="5">
         <v>21</v>
       </c>
@@ -11303,7 +11307,7 @@
         <v>1219</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="24">
+    <row r="26" spans="1:16" ht="24" hidden="1">
       <c r="A26" s="5">
         <v>22</v>
       </c>
@@ -11395,7 +11399,7 @@
         <v>1219</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="24">
+    <row r="28" spans="1:16" ht="24" hidden="1">
       <c r="A28" s="5">
         <v>24</v>
       </c>
@@ -11497,11 +11501,11 @@
       <c r="O30" s="5"/>
       <c r="P30" s="5"/>
     </row>
-    <row r="31" spans="1:16" ht="24">
+    <row r="31" spans="1:16" ht="24" hidden="1">
       <c r="A31" s="59">
         <v>25</v>
       </c>
-      <c r="B31" s="59" t="s">
+      <c r="B31" s="16" t="s">
         <v>136</v>
       </c>
       <c r="C31" s="59" t="s">
@@ -11510,7 +11514,7 @@
       <c r="D31" s="59">
         <v>25.1</v>
       </c>
-      <c r="E31" s="59" t="s">
+      <c r="E31" s="16" t="s">
         <v>133</v>
       </c>
       <c r="F31" s="59" t="s">
@@ -11556,15 +11560,15 @@
     <hyperlink ref="H22" r:id="rId9" display="http://nestuat.tradesmartonline.in/NestHtml5Mobile/rest/Holding"/>
     <hyperlink ref="H25" r:id="rId10" display="http://nestuat.tradesmartonline.in/NestHtml5Mobile/rest/UserProfile"/>
     <hyperlink ref="H10" r:id="rId11" display="http://nestuat.tradesmartonline.in/NestHtml5Mobile/rest/DefaultLogin"/>
-    <hyperlink ref="H7" r:id="rId12" display="http://nestuat.tradesmartonline.in/NestHtml5Mobile/rest/Login2FA&#10;"/>
-    <hyperlink ref="G2" r:id="rId13" display="http://52.43.99.16:8000/get_initial_token/"/>
-    <hyperlink ref="G7" r:id="rId14" display="http://52.43.99.16:8000/login_2fa/"/>
-    <hyperlink ref="G16" r:id="rId15" display="http://127.0.0.1:8000/place_order/"/>
-    <hyperlink ref="G17" r:id="rId16" display="http://52.43.99.16:8000/order_book/"/>
-    <hyperlink ref="G18" r:id="rId17" display="http://52.43.99.16:8000/modify_order/"/>
-    <hyperlink ref="G31" r:id="rId18" display="http://127.0.0.1:8000/logout/"/>
-    <hyperlink ref="H4" r:id="rId19"/>
-    <hyperlink ref="H2" r:id="rId20" display="http://nestuat.tradesmartonline.in/NestHtml5Mobile/rest/GetInitialKey"/>
+    <hyperlink ref="G2" r:id="rId12" display="http://52.43.99.16:8000/get_initial_token/"/>
+    <hyperlink ref="G16" r:id="rId13" display="http://127.0.0.1:8000/place_order/"/>
+    <hyperlink ref="G17" r:id="rId14" display="http://52.43.99.16:8000/order_book/"/>
+    <hyperlink ref="G18" r:id="rId15" display="http://52.43.99.16:8000/modify_order/"/>
+    <hyperlink ref="G31" r:id="rId16" display="http://127.0.0.1:8000/logout/"/>
+    <hyperlink ref="H4" r:id="rId17"/>
+    <hyperlink ref="H2" r:id="rId18" display="http://nestuat.tradesmartonline.in/NestHtml5Mobile/rest/GetInitialKey"/>
+    <hyperlink ref="G7" r:id="rId19" display="http://52.43.99.16:8000/login_2fa/"/>
+    <hyperlink ref="H7" r:id="rId20" display="http://nestuat.tradesmartonline.in/NestHtml5Mobile/rest/Login2FA&#10;"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId21"/>
@@ -13770,10 +13774,10 @@
   <dimension ref="A1:P107"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I33" sqref="I33"/>
+      <selection pane="bottomRight" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -17006,10 +17010,10 @@
   <dimension ref="A1:K371"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E124" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A355" sqref="A355:XFD371"/>
+      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -26458,10 +26462,10 @@
   <dimension ref="A1:G119"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E75" sqref="E75"/>
+      <selection pane="bottomRight" activeCell="A17" sqref="A12:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -31934,7 +31938,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>